<commit_message>
Initial commit from VSCode
</commit_message>
<xml_diff>
--- a/Checkpoints/Checkpoints.xlsx
+++ b/Checkpoints/Checkpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meghp\Desktop\Ahmedabad University\Term 1\Artificial Intelligence Lab\Bird Species Detection\Checkpoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2366437A-7AA7-475E-A9CD-61DF53E53417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5472354E-6727-4E05-892A-F3FD6A990D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update README.md with project description and table of contents
</commit_message>
<xml_diff>
--- a/Checkpoints/Checkpoints.xlsx
+++ b/Checkpoints/Checkpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meghp\Desktop\Ahmedabad University\Term 1\Artificial Intelligence Lab\Bird Species Detection\Checkpoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5472354E-6727-4E05-892A-F3FD6A990D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDCF715-8DA0-4A4A-A3F6-9904E31A2F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,8 @@
   <si>
     <t>1. Updated classes.txt file manually
 2. Updated image_class_labels.txt file in the dataset as per the selected species using pandas functions [Conversion of the txt files to csv files and making updates through functions, and then again converting the csv back to txt file]
-3. Updated images.txt file manually</t>
+3. Updated images.txt file manually
+4. Deleted folders for the species which are not considered</t>
   </si>
 </sst>
 </file>
@@ -498,7 +499,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45916</v>
       </c>

</xml_diff>

<commit_message>
Update Checkpoints.xlsx with latest progress data
</commit_message>
<xml_diff>
--- a/Checkpoints/Checkpoints.xlsx
+++ b/Checkpoints/Checkpoints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meghp\Desktop\Ahmedabad University\Term 1\Artificial Intelligence Lab\Bird Species Detection\Checkpoints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meghp\Desktop\Ahmedabad University\Term 1\CSE618 Artificial Intelligence Laboratory\Bird Species Detection\Checkpoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDCF715-8DA0-4A4A-A3F6-9904E31A2F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6540DF9C-10C9-4BA9-891E-BFDEC8175877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -78,13 +78,16 @@
 2. Updated image_class_labels.txt file in the dataset as per the selected species using pandas functions [Conversion of the txt files to csv files and making updates through functions, and then again converting the csv back to txt file]
 3. Updated images.txt file manually
 4. Deleted folders for the species which are not considered</t>
+  </si>
+  <si>
+    <t>Get the range of the number of species for all the species considered/non-considered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,11 +115,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Montserrat"/>
     </font>
     <font>
       <b/>
@@ -157,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -180,11 +178,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,10 +245,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -496,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,10 +548,11 @@
     <col min="4" max="4" width="86.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="71.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="37.799999999999997" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -522,8 +561,9 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -542,8 +582,11 @@
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>45915</v>
       </c>
@@ -562,8 +605,9 @@
       <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45916</v>
       </c>
@@ -581,11 +625,14 @@
       </c>
       <c r="F4" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>